<commit_message>
excel compare version changed
</commit_message>
<xml_diff>
--- a/Excel Files/TestWorkbook.xlsx
+++ b/Excel Files/TestWorkbook.xlsx
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
   <si>
     <t>e</t>
@@ -369,37 +363,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "excel compare version changed"
This reverts commit ffe6074d0c9952b8855490b02d5f38bc86dc20f4.
</commit_message>
<xml_diff>
--- a/Excel Files/TestWorkbook.xlsx
+++ b/Excel Files/TestWorkbook.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
   <si>
     <t>e</t>
@@ -363,43 +369,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>